<commit_message>
fix a typo in the entry
</commit_message>
<xml_diff>
--- a/Data/Sachdeva_Final_datasheet_OCT_metabolic_232023.xlsx
+++ b/Data/Sachdeva_Final_datasheet_OCT_metabolic_232023.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11113"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D0009DE3-55F3-9B4D-9938-E1F659EAC938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1415530-588B-064B-A5C4-B373829DA0B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6580" yWindow="3800" windowWidth="22260" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6320" yWindow="2680" windowWidth="22260" windowHeight="15860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
   <si>
     <t>age</t>
   </si>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t>LDL</t>
-  </si>
-  <si>
-    <t>114. 729</t>
   </si>
   <si>
     <t>Triglycerides</t>
@@ -516,7 +513,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -568,6 +565,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -851,10 +851,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DH41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BC1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="CW1" sqref="CW1"/>
-      <selection pane="bottomLeft" activeCell="BP1" sqref="BP1"/>
+      <selection pane="bottomLeft" activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -963,7 +963,7 @@
   <sheetData>
     <row r="1" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -975,16 +975,16 @@
         <v>1</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>92</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>5</v>
@@ -993,7 +993,7 @@
         <v>4</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L1" s="10" t="s">
         <v>6</v>
@@ -1002,301 +1002,301 @@
         <v>7</v>
       </c>
       <c r="N1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="R1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="S1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="R1" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="S1" s="11" t="s">
+      <c r="U1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="U1" s="7" t="s">
+      <c r="V1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="W1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="W1" s="12" t="s">
+      <c r="X1" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="X1" s="12" t="s">
+      <c r="Y1" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="Y1" s="15" t="s">
+      <c r="AA1" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="AB1" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="Z1" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA1" s="12" t="s">
+      <c r="AC1" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD1" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE1" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF1" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="AB1" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="AC1" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="AD1" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="AE1" s="12" t="s">
+      <c r="AG1" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="AF1" s="14" t="s">
+      <c r="AH1" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="AI1" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="AJ1" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AK1" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="AG1" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="AH1" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="AI1" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="AJ1" s="12" t="s">
+      <c r="AL1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="AK1" s="14" t="s">
+      <c r="AM1" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="AN1" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="AO1" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="AP1" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="AL1" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="AM1" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="AN1" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="AO1" s="12" t="s">
+      <c r="AQ1" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="AP1" s="14" t="s">
+      <c r="AR1" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AS1" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="AT1" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="AU1" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="AQ1" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="AR1" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="AS1" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="AT1" s="12" t="s">
+      <c r="AV1" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="AU1" s="14" t="s">
+      <c r="AW1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="AX1" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="AY1" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="AZ1" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="AV1" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="AW1" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="AX1" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="AY1" s="12" t="s">
+      <c r="BA1" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="AZ1" s="14" t="s">
+      <c r="BB1" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="BC1" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="BD1" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="BE1" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="BA1" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="BB1" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="BC1" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="BD1" s="12" t="s">
+      <c r="BF1" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="BE1" s="14" t="s">
+      <c r="BG1" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="BH1" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="BI1" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="BJ1" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="BF1" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="BG1" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="BH1" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="BI1" s="12" t="s">
+      <c r="BK1" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="BJ1" s="12" t="s">
+      <c r="BL1" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="BM1" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="BN1" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="BO1" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="BK1" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="BL1" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="BM1" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="BN1" s="12" t="s">
+      <c r="BP1" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="BO1" s="14" t="s">
+      <c r="BQ1" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="BR1" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="BS1" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="BT1" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="BP1" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="BQ1" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="BR1" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="BS1" s="16" t="s">
+      <c r="BU1" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="BT1" s="17" t="s">
+      <c r="BV1" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="BW1" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="BX1" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="BY1" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="BU1" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="BV1" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="BW1" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="BX1" s="16" t="s">
+      <c r="BZ1" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="BY1" s="17" t="s">
+      <c r="CA1" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="CB1" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="CC1" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="CD1" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="BZ1" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="CA1" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="CB1" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="CC1" s="17" t="s">
+      <c r="CE1" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="CD1" s="17" t="s">
+      <c r="CF1" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="CG1" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="CH1" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="CI1" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="CE1" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="CF1" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="CG1" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="CH1" s="16" t="s">
+      <c r="CJ1" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="CI1" s="17" t="s">
+      <c r="CK1" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="CL1" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="CM1" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="CN1" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="CJ1" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="CK1" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="CL1" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="CM1" s="16" t="s">
+      <c r="CO1" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="CN1" s="17" t="s">
+      <c r="CP1" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="CQ1" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="CR1" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="CS1" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="CO1" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="CP1" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="CQ1" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="CR1" s="16" t="s">
+      <c r="CT1" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="CS1" s="17" t="s">
+      <c r="CU1" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="CV1" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="CW1" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="CX1" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="CT1" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="CU1" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="CV1" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="CW1" s="16" t="s">
+      <c r="CY1" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="CX1" s="17" t="s">
+      <c r="CZ1" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="DA1" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="DB1" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="DC1" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="CY1" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="CZ1" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="DA1" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="DB1" s="16" t="s">
+      <c r="DD1" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="DC1" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="DD1" s="16" t="s">
+      <c r="DE1" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="DE1" s="16" t="s">
+      <c r="DF1" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="DF1" s="17" t="s">
+      <c r="DG1" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="DG1" s="16" t="s">
+      <c r="DH1" s="17" t="s">
         <v>89</v>
-      </c>
-      <c r="DH1" s="17" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:112" x14ac:dyDescent="0.2">
@@ -4871,8 +4871,8 @@
       <c r="M13" s="3">
         <v>73</v>
       </c>
-      <c r="N13" s="4" t="s">
-        <v>8</v>
+      <c r="N13" s="18">
+        <v>114.729</v>
       </c>
       <c r="O13" s="3">
         <v>189.761</v>

</xml_diff>